<commit_message>
Added commentation, linux  fileslashes
</commit_message>
<xml_diff>
--- a/ilm.xlsx
+++ b/ilm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UT\git\UT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0917FF7-DBE4-47B9-AAAE-5670265252B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2F6740-56D3-4ECE-B95A-11B2AC77EC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Outside Temperature</t>
   </si>
@@ -71,57 +71,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>18.3C</t>
-  </si>
-  <si>
-    <t>18.5C</t>
-  </si>
-  <si>
-    <t>16.0C</t>
-  </si>
-  <si>
-    <t>86%</t>
-  </si>
-  <si>
-    <t>1003.4 mbar (1.0)</t>
-  </si>
-  <si>
-    <t>0.5 m/s ESE (121)</t>
-  </si>
-  <si>
-    <t>0.0 mm/h</t>
-  </si>
-  <si>
-    <t>1.0 mm</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>0.0 mm</t>
-  </si>
-  <si>
-    <t>274 W/m2</t>
-  </si>
-  <si>
-    <t>23.0C</t>
-  </si>
-  <si>
-    <t>53%</t>
-  </si>
-  <si>
-    <t>0.632</t>
-  </si>
-  <si>
-    <t>12:21</t>
-  </si>
-  <si>
-    <t>05-07</t>
-  </si>
-  <si>
-    <t>12:22</t>
   </si>
 </sst>
 </file>
@@ -170,42 +119,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -265,22 +184,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -566,267 +483,171 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.9296875" customWidth="1"/>
-    <col min="6" max="6" width="16.53125" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="30.265625" customWidth="1"/>
-    <col min="9" max="9" width="31.06640625" customWidth="1"/>
+    <col min="1" max="1" width="20.265625" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" customWidth="1"/>
+    <col min="4" max="4" width="9.53125" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.3984375" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.796875" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.86328125" customWidth="1"/>
+    <col min="15" max="15" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="2"/>
       <c r="T1" s="1"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>32</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>32</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="6"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test if new excel works, 02.01.2025 18:24
</commit_message>
<xml_diff>
--- a/ilm.xlsx
+++ b/ilm.xlsx
@@ -1,119 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tanel\Desktop\UT-1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F9D60D-A594-4382-AC6F-75E811624C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11423" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Outside Temperature</t>
-  </si>
-  <si>
-    <t>Heat Index</t>
-  </si>
-  <si>
-    <t>Wind Chill</t>
-  </si>
-  <si>
-    <t>Dew Point</t>
-  </si>
-  <si>
-    <t>Humidity</t>
-  </si>
-  <si>
-    <t>Barometer</t>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Rain Rate</t>
-  </si>
-  <si>
-    <t>Rain Today</t>
-  </si>
-  <si>
-    <t>UV Index</t>
-  </si>
-  <si>
-    <t>ET</t>
-  </si>
-  <si>
-    <t>Radiation</t>
-  </si>
-  <si>
-    <t>Inside Temperature</t>
-  </si>
-  <si>
-    <t>Inside Humidity</t>
-  </si>
-  <si>
-    <t>Elektrihind</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -147,42 +86,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -448,136 +446,243 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.265625" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" customWidth="1"/>
-    <col min="4" max="4" width="9.53125" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.3984375" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.796875" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.86328125" customWidth="1"/>
-    <col min="15" max="15" width="9.73046875" customWidth="1"/>
+    <col width="20.265625" customWidth="1" min="1" max="1"/>
+    <col width="10.86328125" customWidth="1" min="2" max="2"/>
+    <col width="10.73046875" customWidth="1" min="3" max="3"/>
+    <col width="9.53125" customWidth="1" min="4" max="4"/>
+    <col width="12.33203125" customWidth="1" min="6" max="6"/>
+    <col width="12.3984375" customWidth="1" min="7" max="7"/>
+    <col width="17.6640625" customWidth="1" min="8" max="8"/>
+    <col width="18.796875" customWidth="1" min="9" max="9"/>
+    <col width="19.33203125" customWidth="1" min="13" max="13"/>
+    <col width="13.86328125" customWidth="1" min="14" max="14"/>
+    <col width="9.73046875" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="6"/>
-      <c r="T1" s="7"/>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Outside Temperature</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Heat Index</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Wind Chill</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Dew Point</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Humidity</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Barometer</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Wind</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Rain Rate</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Rain Today</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>UV Index</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>ET</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>Radiation</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>Inside Temperature</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
+        <is>
+          <t>Inside Humidity</t>
+        </is>
+      </c>
+      <c r="O1" s="5" t="inlineStr">
+        <is>
+          <t>Elektrihind</t>
+        </is>
+      </c>
+      <c r="P1" s="4" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="Q1" s="4" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="R1" s="6" t="n"/>
+      <c r="T1" s="7" t="n"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>-3.8C</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>-3.8C</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>-3.8C</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>-3.9C</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>99%</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>992.8 mbar (0.9)</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>0.1 m/s E (82)</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>0.0 mm/h</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>0.0 mm</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>0.0 mm</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>0 W/m2</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>22.5C</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>29%</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>15.199</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>02-01</t>
+        </is>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+    <row r="3">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="n"/>
+      <c r="J3" s="3" t="n"/>
+      <c r="K3" s="3" t="n"/>
+      <c r="L3" s="3" t="n"/>
+      <c r="M3" s="3" t="n"/>
+      <c r="N3" s="3" t="n"/>
+      <c r="O3" s="3" t="n"/>
+      <c r="P3" s="3" t="n"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+    <row r="6">
+      <c r="A6" s="2" t="n"/>
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="2" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="2" t="n"/>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+      <c r="N6" s="2" t="n"/>
+      <c r="O6" s="2" t="n"/>
+      <c r="P6" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>